<commit_message>
Update on 29 Sep 2017
</commit_message>
<xml_diff>
--- a/horizon/xl_datasheets/48006/48006_new_asldfkj_alsdnvla.xlsx
+++ b/horizon/xl_datasheets/48006/48006_new_asldfkj_alsdnvla.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="new_asldfkj alsdnvla" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -28,7 +28,10 @@
     <t xml:space="preserve">V</t>
   </si>
   <si>
-    <t xml:space="preserve">Place</t>
+    <t xml:space="preserve">Place1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place2</t>
   </si>
   <si>
     <t xml:space="preserve">Q2 (Ton)</t>
@@ -40,7 +43,22 @@
     <t xml:space="preserve">Quantum Logistics</t>
   </si>
   <si>
-    <t xml:space="preserve">Location1</t>
+    <t xml:space="preserve">Shanghai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ningbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/7/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nanjing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/7/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzhou</t>
   </si>
   <si>
     <t xml:space="preserve">2017/7/3</t>
@@ -49,22 +67,16 @@
     <t xml:space="preserve">2017/7/4</t>
   </si>
   <si>
-    <t xml:space="preserve">Location2</t>
-  </si>
-  <si>
     <t xml:space="preserve">2017/7/5</t>
   </si>
   <si>
+    <t xml:space="preserve">Quantum SCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guangzhou</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017/7/6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017/7/7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantum SCM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017/7/8</t>
   </si>
 </sst>
 </file>
@@ -162,15 +174,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7894736842105"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -189,22 +203,28 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>7</v>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -212,16 +232,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -229,16 +252,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,49 +272,53 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
+      <c r="F7" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 12 Nov 2017
</commit_message>
<xml_diff>
--- a/horizon/xl_datasheets/48006/48006_new_asldfkj_alsdnvla.xlsx
+++ b/horizon/xl_datasheets/48006/48006_new_asldfkj_alsdnvla.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="new_asldfkj alsdnvla" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,24 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t xml:space="preserve">#</t>
   </si>
   <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2 (Ton)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
+    <t xml:space="preserve">Vendor Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trips</t>
   </si>
   <si>
     <t xml:space="preserve">Quantum Logistics</t>
@@ -49,34 +49,16 @@
     <t xml:space="preserve">Ningbo</t>
   </si>
   <si>
-    <t xml:space="preserve">2017/7/1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nanjing</t>
   </si>
   <si>
-    <t xml:space="preserve">2017/7/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Suzhou</t>
   </si>
   <si>
-    <t xml:space="preserve">2017/7/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017/7/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017/7/5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantum SCM</t>
   </si>
   <si>
     <t xml:space="preserve">Guangzhou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017/7/6</t>
   </si>
 </sst>
 </file>
@@ -177,14 +159,12 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7894736842105"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,8 +203,8 @@
       <c r="E2" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
+      <c r="F2" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,13 +218,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1500</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,7 +235,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -263,8 +243,8 @@
       <c r="E4" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>13</v>
+      <c r="F4" s="0" t="n">
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,8 +263,8 @@
       <c r="E5" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>14</v>
+      <c r="F5" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,7 +272,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
@@ -300,16 +280,16 @@
       <c r="E6" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>15</v>
+      <c r="F6" s="0" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
@@ -317,8 +297,8 @@
       <c r="E7" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>18</v>
+      <c r="F7" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>